<commit_message>
Úprava precedence_table a začátek bottom_up funkce
</commit_message>
<xml_diff>
--- a/ifj21_precedence_table.xlsx
+++ b/ifj21_precedence_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seiti\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IFJ\IFJ21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F26F82-2820-4593-9ACD-C8B4BCAA8BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C637A17C-361C-49FA-ADA0-656ABF432126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="4230" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="14">
   <si>
     <t>Precedenční tabulka</t>
   </si>
@@ -67,26 +67,23 @@
     <t>+ -</t>
   </si>
   <si>
-    <t>Finish</t>
-  </si>
-  <si>
     <t>&lt;</t>
   </si>
   <si>
-    <t>Err</t>
-  </si>
-  <si>
     <t>&gt;</t>
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,16 +91,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -384,11 +394,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,9 +439,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -447,6 +466,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,8 +494,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Špatně" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -739,7 +777,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,18 +787,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
@@ -770,7 +808,7 @@
       <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -797,32 +835,30 @@
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>13</v>
+      <c r="B3" s="21"/>
+      <c r="C3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -830,65 +866,65 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>11</v>
+      <c r="B4" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>11</v>
+      <c r="B5" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -896,32 +932,32 @@
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>11</v>
+      <c r="B6" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -929,32 +965,32 @@
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>11</v>
+      <c r="B7" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -962,65 +998,57 @@
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>11</v>
+      <c r="B8" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>12</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>12</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J8" s="20"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="B9" s="22"/>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G9" s="19"/>
       <c r="H9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I9" s="19"/>
+      <c r="J9" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="K9" s="1"/>
     </row>
@@ -1028,32 +1056,28 @@
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>13</v>
+      <c r="B10" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G10" s="19"/>
       <c r="H10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="I10" s="19"/>
+      <c r="J10" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="K10" s="1"/>
     </row>
@@ -1061,32 +1085,30 @@
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>10</v>
+      <c r="B11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="K11" s="1"/>
     </row>

</xml_diff>